<commit_message>
Updated Chapters 1-3 and 10, plus new appendices
</commit_message>
<xml_diff>
--- a/data/demo.xlsx
+++ b/data/demo.xlsx
@@ -417,7 +417,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="2">
-        <v>45405</v>
+        <v>45957</v>
       </c>
     </row>
     <row r="3">
@@ -441,7 +441,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>45404</v>
+        <v>45956</v>
       </c>
     </row>
     <row r="4">
@@ -465,7 +465,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>45403</v>
+        <v>45955</v>
       </c>
     </row>
     <row r="5">
@@ -489,7 +489,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>45402</v>
+        <v>45954</v>
       </c>
     </row>
     <row r="6">
@@ -510,7 +510,7 @@
         <v>5.5</v>
       </c>
       <c r="F6" s="2">
-        <v>45401</v>
+        <v>45953</v>
       </c>
     </row>
     <row r="7">
@@ -534,7 +534,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="2">
-        <v>45400</v>
+        <v>45952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>